<commit_message>
remove node hard code
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="83">
   <si>
     <t>id</t>
   </si>
@@ -1216,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1235,7 +1235,7 @@
     <col min="11" max="11" width="17.7265625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1269,8 +1269,11 @@
       <c r="K1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1304,8 +1307,11 @@
       <c r="K2" s="8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1325,7 +1331,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="67" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="67" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1348,7 +1354,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1362,7 +1368,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1373,7 +1379,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1384,7 +1390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1395,7 +1401,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1406,7 +1412,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1417,7 +1423,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1428,7 +1434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1439,7 +1445,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1450,7 +1456,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1461,7 +1467,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
handle exception and add APIs
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OrgChart\project\Dagre-d3\orgchart\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21790" windowHeight="5250" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7230" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Structures" sheetId="1" r:id="rId1"/>
@@ -13,9 +18,9 @@
     <sheet name="Competence master data" sheetId="4" r:id="rId4"/>
     <sheet name="Possition" sheetId="5" r:id="rId5"/>
     <sheet name="Domain" sheetId="6" r:id="rId6"/>
+    <sheet name="Career Path" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:V18"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="94">
   <si>
     <t>id</t>
   </si>
@@ -108,10 +113,6 @@
   </si>
   <si>
     <t>P1, P2, P3,P4</t>
-  </si>
-  <si>
-    <t>&lt;refer competence master data&gt;
-&lt;each of competence is one line&gt;</t>
   </si>
   <si>
     <t>&lt;free text&gt;</t>
@@ -265,17 +266,98 @@
     <t>DQA</t>
   </si>
   <si>
+    <t>IT</t>
+  </si>
+  <si>
     <t>Principal Consultant</t>
   </si>
   <si>
-    <t>IT</t>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Career path</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Domain Roles</t>
+  </si>
+  <si>
+    <t>Project Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competencies required </t>
+  </si>
+  <si>
+    <t>KRA (key responsible area)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scope </t>
+  </si>
+  <si>
+    <t>Responsibilities</t>
+  </si>
+  <si>
+    <t>Industrial Role</t>
+  </si>
+  <si>
+    <t>Entry Criteria</t>
+  </si>
+  <si>
+    <t>KRA1</t>
+  </si>
+  <si>
+    <t>KRA2</t>
+  </si>
+  <si>
+    <t>KRA3</t>
+  </si>
+  <si>
+    <t>KRA4</t>
+  </si>
+  <si>
+    <t>KRA5</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>Career Path</t>
+  </si>
+  <si>
+    <t>#0E78C5</t>
+  </si>
+  <si>
+    <t>#1399A0</t>
+  </si>
+  <si>
+    <t>#67B419</t>
+  </si>
+  <si>
+    <t>#5b2287</t>
+  </si>
+  <si>
+    <t>#BFBFBF</t>
+  </si>
+  <si>
+    <t>SCP</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>LCP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -307,6 +389,12 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -375,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -405,6 +493,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -921,6 +1012,41 @@
       <c r="I8" s="3"/>
       <c r="J8" s="4"/>
       <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -938,31 +1064,65 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>14</v>
@@ -970,114 +1130,129 @@
       <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="7">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>17</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="67" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
+      <c r="B4">
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="G4" s="9">
+        <v>4</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="I4" s="9"/>
       <c r="J4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
+      <c r="B6">
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>27</v>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D5">
-      <formula1>$R$1:$R$11</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1087,23 +1262,26 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,13 +1289,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1125,13 +1303,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1139,13 +1317,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1153,13 +1331,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1167,13 +1345,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1181,27 +1359,27 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="11">
-        <v>2</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>7</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="11">
-        <v>2</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>39</v>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1211,26 +1389,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="25.08984375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>2</v>
@@ -1241,10 +1416,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="D2" s="12">
         <v>1</v>
@@ -1255,10 +1430,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="D3" s="12">
         <v>1</v>
@@ -1269,10 +1444,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
@@ -1283,10 +1458,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="12">
         <v>2</v>
@@ -1297,10 +1472,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="12">
         <v>2</v>
@@ -1311,37 +1486,26 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>52</v>
-      </c>
       <c r="D7" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="12">
         <v>2</v>
       </c>
     </row>
@@ -1352,26 +1516,33 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.90625" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -1381,8 +1552,11 @@
       <c r="C2" s="14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -1390,10 +1564,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -1401,10 +1578,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -1412,10 +1592,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -1423,10 +1606,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -1434,10 +1620,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -1445,10 +1634,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -1456,10 +1648,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -1467,10 +1662,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -1478,10 +1676,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -1489,10 +1690,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -1500,10 +1704,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -1511,10 +1718,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>14</v>
       </c>
@@ -1522,10 +1732,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>15</v>
       </c>
@@ -1533,10 +1746,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>16</v>
       </c>
@@ -1544,10 +1760,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -1555,18 +1774,24 @@
         <v>1</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+        <v>64</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="14">
-        <v>1</v>
-      </c>
-      <c r="C19" s="14" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>66</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1584,7 +1809,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1602,18 +1827,100 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added for add connection api
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRA81HC\Desktop\WorkPlace\Repositories\bosch-git\Newfolder\orgchart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRA81HC\Desktop\WorkPlace\Repositories\bosch-git\Newfolder\RoleNxtAPIs\target\classes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="110">
   <si>
     <t>id</t>
   </si>
@@ -1593,10 +1593,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1772,12 +1772,8 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="F12" s="19">
-        <v>10</v>
-      </c>
-      <c r="G12" s="19">
-        <v>11</v>
-      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
@@ -1792,12 +1788,8 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="F13" s="19">
-        <v>10</v>
-      </c>
-      <c r="G13" s="19">
-        <v>13</v>
-      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
@@ -1812,12 +1804,8 @@
       <c r="D14">
         <v>2</v>
       </c>
-      <c r="F14" s="19">
-        <v>11</v>
-      </c>
-      <c r="G14" s="19">
-        <v>14</v>
-      </c>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
@@ -1832,12 +1820,8 @@
       <c r="D15">
         <v>2</v>
       </c>
-      <c r="F15" s="19">
-        <v>11</v>
-      </c>
-      <c r="G15" s="19">
-        <v>7</v>
-      </c>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
@@ -1981,6 +1965,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
+        <f>A25+1</f>
         <v>25</v>
       </c>
       <c r="B26" s="14">
@@ -1991,6 +1976,141 @@
       </c>
       <c r="D26">
         <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
+        <f t="shared" ref="A27:A35" si="0">A26+1</f>
+        <v>26</v>
+      </c>
+      <c r="B27" s="14">
+        <v>2</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="18">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="14">
+        <v>2</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="18">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="14">
+        <v>2</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="14">
+        <v>2</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="14">
+        <v>2</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="18">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="14">
+        <v>2</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="14">
+        <v>2</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="18">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="14">
+        <v>2</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="14">
+        <v>2</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2124,8 +2244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>